<commit_message>
Update experiments, leaving keyword
</commit_message>
<xml_diff>
--- a/experiment.xlsx
+++ b/experiment.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Baseline</t>
   </si>
@@ -45,9 +45,6 @@
   <si>
     <t>Reranking
 (Not stable for TFIDF)  + Rewriting + Direct Match</t>
-  </si>
-  <si>
-    <t>Rewriting + Direct Match</t>
   </si>
   <si>
     <t>TF-IDF</t>
@@ -128,6 +125,14 @@
 Fuzzy doc search count: 44, hit count: 31, rate: 0.705</t>
   </si>
   <si>
+    <t>Accuracy: 0.86
+Time taken: 46.5548620223999
+Direct match count: 56
+Full chain count: 44
+Explicit doc search count: 56, hit count: 55, rate: 0.982
+Fuzzy doc search count: 44, hit count: 31, rate: 0.705</t>
+  </si>
+  <si>
     <t>Hybrid(0.5, 0.5)</t>
   </si>
   <si>
@@ -171,12 +176,103 @@
 Fuzzy doc search count: 44, hit count: 26, rate: 0.591</t>
   </si>
   <si>
-    <t>Accuracy: 0.81
-Time taken: 38.399900913238525
-Direct match count: 56
-Full chain count: 44
-Explicit doc search count: 56, hit count: 55, rate: 0.982
-Fuzzy doc search count: 44, hit count: 26, rate: 0.591</t>
+    <t>TF-IDF
+(With Rewriting)</t>
+  </si>
+  <si>
+    <t>37242 dimension</t>
+  </si>
+  <si>
+    <t>10000 dimension</t>
+  </si>
+  <si>
+    <t>5000 dimension</t>
+  </si>
+  <si>
+    <t>1000 dimension</t>
+  </si>
+  <si>
+    <t>30 dimension</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.49
+Time taken: 1540.9216396808624
+Direct match count: 0
+Full chain count: 100
+Explicit doc search count: 56, hit count: 26, rate: 0.464
+Fuzzy doc search count: 44, hit count: 23, rate: 0.523</t>
+  </si>
+  <si>
+    <t>Hit count: 42
+Total: 100
+Accuracy: 0.42
+Time taken: 1168.9623773097992</t>
+  </si>
+  <si>
+    <t>Hit count: 33
+Total: 100
+Accuracy: 0.33
+Time taken: 778.6862154006958</t>
+  </si>
+  <si>
+    <t>Hit count: 18
+Total: 100
+Accuracy: 0.18
+Time taken: 86.76330947875977</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.0
+Time taken: 42.70797538757324
+Direct match count: 0
+Full chain count: 100
+Explicit doc search count: 56, hit count: 0, rate: 0.000
+Fuzzy doc search count: 44, hit count: 0, rate: 0.000</t>
+  </si>
+  <si>
+    <t>Vector
+(With Rewriting)</t>
+  </si>
+  <si>
+    <t>1536 dimension</t>
+  </si>
+  <si>
+    <t>768 dimension</t>
+  </si>
+  <si>
+    <t>384 dimension</t>
+  </si>
+  <si>
+    <t>100 dimension</t>
+  </si>
+  <si>
+    <t>Hit count: 42
+Total: 100
+Accuracy: 0.42
+Time taken: 110.6396918296814</t>
+  </si>
+  <si>
+    <t>Hit count: 42
+Total: 100
+Accuracy: 0.42
+Time taken: 40.57761836051941</t>
+  </si>
+  <si>
+    <t>Hit count: 41
+Total: 100
+Accuracy: 0.41
+Time taken: 41.47486901283264</t>
+  </si>
+  <si>
+    <t>Hit count: 32
+Total: 100
+Accuracy: 0.32
+Time taken: 40.96525311470032</t>
+  </si>
+  <si>
+    <t>Accuracy: 0.1
+Time taken: 85.96082067489624
+Direct match count: 0
+Full chain count: 100</t>
   </si>
 </sst>
 </file>
@@ -348,18 +444,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -680,7 +770,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -704,16 +794,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -722,85 +812,85 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -820,13 +910,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1354,26 +1444,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="16.3076923076923" style="1" customWidth="1"/>
     <col min="2" max="2" width="57.3653846153846" style="2" customWidth="1"/>
     <col min="3" max="3" width="50.4807692307692" style="1" customWidth="1"/>
     <col min="4" max="4" width="62.9423076923077" style="1" customWidth="1"/>
-    <col min="5" max="7" width="49.2307692307692" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.23076923076923" style="1"/>
+    <col min="5" max="6" width="49.2307692307692" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.23076923076923" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="34" spans="2:7">
-      <c r="B1" s="2" t="s">
+    <row r="1" ht="34" spans="2:6">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1388,51 +1478,48 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+    </row>
+    <row r="2" ht="105" customHeight="1" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" ht="105" customHeight="1" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="6" t="s">
+    <row r="3" ht="108" customHeight="1" spans="1:6">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" ht="108" customHeight="1" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" ht="101" spans="1:7">
+    <row r="4" ht="101" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1450,15 +1537,90 @@
       </c>
       <c r="F4" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" s="4"/>
     </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" ht="101" spans="2:6">
+      <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" ht="68" spans="2:6">
+      <c r="B12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>